<commit_message>
cadastro e visualização ok
</commit_message>
<xml_diff>
--- a/bank/itens.xlsx
+++ b/bank/itens.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,10 +476,8 @@
           <t>testeee</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
+      <c r="D2" t="n">
+        <v>8</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -503,15 +501,38 @@
           <t>asas</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
+      <c r="D3" t="n">
+        <v>25</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
           <t>s</t>
         </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>laizer</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>0858-05-08</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>8585</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>858</t>
+        </is>
+      </c>
+      <c r="E4" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
todas as func ok, falta mais tela de user
</commit_message>
<xml_diff>
--- a/bank/itens.xlsx
+++ b/bank/itens.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,74 +459,38 @@
           <t>Urgencia</t>
         </is>
       </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>teste</t>
-        </is>
+      <c r="A2" t="n">
+        <v>99</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>58555-08-05</t>
+          <t>0008-08-08</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>galinha</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>8</v>
+          <t>t de 2</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
       </c>
       <c r="E2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>eraudo</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>85855-05-08</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>laps</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>25</v>
-      </c>
-      <c r="E3" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>laizer</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>0858-05-08</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>8585</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
-        <v>858</v>
-      </c>
-      <c r="E4" t="b">
-        <v>0</v>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Expedição</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>